<commit_message>
Update seeding of UserOnOrg
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26605"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE1EB751-C54B-4CD8-A755-44DD6BE978AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F86172FB-BE60-4EB0-9D49-4367019E5505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seeding Instruction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="637">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -97,85 +97,85 @@
     <t>NUSC Management Committee</t>
   </si>
   <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Gautham</t>
+  </si>
+  <si>
+    <t>Celest</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Fiqri</t>
+  </si>
+  <si>
+    <t>Wyman</t>
+  </si>
+  <si>
+    <t>ERICA SOH KE MIN</t>
+  </si>
+  <si>
+    <t>ASHLEY LOW JIA SHUEN</t>
+  </si>
+  <si>
+    <t>WONG ZHI MIN, OLIVIA</t>
+  </si>
+  <si>
+    <t>DUANGPORN SIRIKULWATTANON</t>
+  </si>
+  <si>
+    <t>GILLIAN RAE ANG TIAN-EN</t>
+  </si>
+  <si>
+    <t>EU SHAE-ANNE</t>
+  </si>
+  <si>
+    <t>CRYSTAL PHUA</t>
+  </si>
+  <si>
+    <t>NGIOW HAN BIN</t>
+  </si>
+  <si>
+    <t>ALDWIN CHIA KUN HAN</t>
+  </si>
+  <si>
+    <t>HANNAH ONG SI EN</t>
+  </si>
+  <si>
+    <t>ARCHIT GOSWAMI</t>
+  </si>
+  <si>
+    <t>Zeyuan</t>
+  </si>
+  <si>
+    <t>Rachel Lee Rui Qi</t>
+  </si>
+  <si>
+    <t>NUSC Productions</t>
+  </si>
+  <si>
+    <t>Parth</t>
+  </si>
+  <si>
+    <t>Zhi Sheng</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>telegramUserName</t>
+  </si>
+  <si>
+    <t>ChengYi123</t>
+  </si>
+  <si>
     <t>Shanna Ng Ann Qi</t>
-  </si>
-  <si>
-    <t>Clara</t>
-  </si>
-  <si>
-    <t>Gautham</t>
-  </si>
-  <si>
-    <t>Celest</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Fiqri</t>
-  </si>
-  <si>
-    <t>Wyman</t>
-  </si>
-  <si>
-    <t>ERICA SOH KE MIN</t>
-  </si>
-  <si>
-    <t>ASHLEY LOW JIA SHUEN</t>
-  </si>
-  <si>
-    <t>WONG ZHI MIN, OLIVIA</t>
-  </si>
-  <si>
-    <t>DUANGPORN SIRIKULWATTANON</t>
-  </si>
-  <si>
-    <t>GILLIAN RAE ANG TIAN-EN</t>
-  </si>
-  <si>
-    <t>EU SHAE-ANNE</t>
-  </si>
-  <si>
-    <t>CRYSTAL PHUA</t>
-  </si>
-  <si>
-    <t>NGIOW HAN BIN</t>
-  </si>
-  <si>
-    <t>ALDWIN CHIA KUN HAN</t>
-  </si>
-  <si>
-    <t>HANNAH ONG SI EN</t>
-  </si>
-  <si>
-    <t>ARCHIT GOSWAMI</t>
-  </si>
-  <si>
-    <t>Zeyuan</t>
-  </si>
-  <si>
-    <t>Rachel Lee Rui Qi</t>
-  </si>
-  <si>
-    <t>NUSC Productions</t>
-  </si>
-  <si>
-    <t>Parth</t>
-  </si>
-  <si>
-    <t>Zhi Sheng</t>
-  </si>
-  <si>
-    <t>Megan</t>
-  </si>
-  <si>
-    <t>Conrad</t>
-  </si>
-  <si>
-    <t>telegramUserName</t>
-  </si>
-  <si>
-    <t>ChengYi123</t>
   </si>
   <si>
     <t>holygoats</t>
@@ -493,118 +493,118 @@
     <t>Educational workshops, discussion events, social events within Cinnamon, film screenings</t>
   </si>
   <si>
+    <t>Message IG Head</t>
+  </si>
+  <si>
+    <t>Deepika</t>
+  </si>
+  <si>
+    <t>acsdeepika</t>
+  </si>
+  <si>
+    <t>e0421285@u.nus.edu</t>
+  </si>
+  <si>
+    <t>Livecore</t>
+  </si>
+  <si>
+    <t>Livecore is a continuation of the USP IG of the same name, a group formed for people to come together and play music in the contemporary band format. We play all genres of music that can be created using the basic instruments of vocals, keyboard, guitar, bass and drums, and we are open to all skill levels of musicianship, even those seeking to learn an instrument from scratch. In Livecore, we believe that musicians grow best with a target in mind, so we encourage members to work towards the end goal of recording or performing their music, where the community provides any necessary technical guidance along the way.</t>
+  </si>
+  <si>
+    <t>Jam sessions (themed or unstructured) every 2 weeks, performance opportunities, workshops to learn instruments or develop play ability.</t>
+  </si>
+  <si>
+    <t>Art Fort, themed sessions, weekly jamming sessions, SOS and EOS performance</t>
+  </si>
+  <si>
+    <t>https://t.me/+7Rb2UKPAr1Q1ZTQ9</t>
+  </si>
+  <si>
+    <t>Joshua Wee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joshweeal </t>
+  </si>
+  <si>
+    <t>joshua.wee.al@u.nus.edu</t>
+  </si>
+  <si>
+    <t>Love, NUSC</t>
+  </si>
+  <si>
+    <t>This proposed interest group (IG) is a continuation of a previous USP IG, Love, USP. Love, NUSC is a mental health interest group that aims to carry out activities to promote the awareness of and practice of mental health activities. At Love, NUSC, we believe that good mental health is a key to general well-being, and to that end, we endeavour to promote mental wellness in the community.</t>
+  </si>
+  <si>
+    <t>Every few weeks</t>
+  </si>
+  <si>
+    <t>Love, USP</t>
+  </si>
+  <si>
+    <t>Moodboard, Mental health and USP related dialogue and speaker sessions</t>
+  </si>
+  <si>
+    <t>Joshua Koh Ze Shao</t>
+  </si>
+  <si>
+    <t>joshua_kzs</t>
+  </si>
+  <si>
+    <t>joshuakzs@u.nus.edu</t>
+  </si>
+  <si>
+    <t>NUSC Astronomical Society</t>
+  </si>
+  <si>
+    <t>An astronomy-based interest group that mainly conducts star-gazing activities at night. The interest group will also provide knowledge to members about the different constellations seen at night and share random facts about our night sky. On occasions where eclipses may be observed, members of the interest group would also gather round to observe and document the sight. This interest group is a continuation of a University Scholars Programme interest group called UStronomy.</t>
+  </si>
+  <si>
+    <t>Whenever the sky looks clear enough to star gaze</t>
+  </si>
+  <si>
+    <t>UStronomy</t>
+  </si>
+  <si>
+    <t>https://t.me/joinchat/k07RzjszkIsyODU1</t>
+  </si>
+  <si>
+    <t>Aldwin Chia Kun Han</t>
+  </si>
+  <si>
+    <t>e0773080@u.nus.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUSC Fellowship </t>
+  </si>
+  <si>
+    <t>As a continuation of USFellowship, the USP Christian Fellowship IG, NUSC Fellowship aims to be a community for Christians in NUSC to study the Bible and find support, and for those seeking to find out more about Christianity to explore the faith.</t>
+  </si>
+  <si>
+    <t>Weekly small groups or IG-wide events, additional external speaker events or get-togethers</t>
+  </si>
+  <si>
+    <t>USFellowship</t>
+  </si>
+  <si>
+    <t>Bible/book studies, worship nights, prayer meetings, sharing by USP profs, Apologetics session</t>
+  </si>
+  <si>
+    <t>https://t.me/+Vmf1PYIiALJlMjJl</t>
+  </si>
+  <si>
+    <t>NUSC Invests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are an IG for students to familiarize better with investing, build knowledge on financial literacy, and build skills for those who would like a career in the invest sector.                       NUSC Invests is an interest group for anyone/everyone who are interested in investing. It is a continuation of a USP interest group: US Invest. NUSC Invests does not provide financial advice, but rather creates a vibrant community that discusses the financial market (stocks, bonds, EFTs, and crypto). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock Analysis/ Virtual Portofolio Management/Movie screenings/etc.           Adhoc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Invest. </t>
+  </si>
+  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Message IG Head</t>
-  </si>
-  <si>
-    <t>Deepika</t>
-  </si>
-  <si>
-    <t>acsdeepika</t>
-  </si>
-  <si>
-    <t>e0421285@u.nus.edu</t>
-  </si>
-  <si>
-    <t>Livecore</t>
-  </si>
-  <si>
-    <t>Livecore is a continuation of the USP IG of the same name, a group formed for people to come together and play music in the contemporary band format. We play all genres of music that can be created using the basic instruments of vocals, keyboard, guitar, bass and drums, and we are open to all skill levels of musicianship, even those seeking to learn an instrument from scratch. In Livecore, we believe that musicians grow best with a target in mind, so we encourage members to work towards the end goal of recording or performing their music, where the community provides any necessary technical guidance along the way.</t>
-  </si>
-  <si>
-    <t>Jam sessions (themed or unstructured) every 2 weeks, performance opportunities, workshops to learn instruments or develop play ability.</t>
-  </si>
-  <si>
-    <t>Art Fort, themed sessions, weekly jamming sessions, SOS and EOS performance</t>
-  </si>
-  <si>
-    <t>https://t.me/+7Rb2UKPAr1Q1ZTQ9</t>
-  </si>
-  <si>
-    <t>Joshua Wee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joshweeal </t>
-  </si>
-  <si>
-    <t>joshua.wee.al@u.nus.edu</t>
-  </si>
-  <si>
-    <t>Love, NUSC</t>
-  </si>
-  <si>
-    <t>This proposed interest group (IG) is a continuation of a previous USP IG, Love, USP. Love, NUSC is a mental health interest group that aims to carry out activities to promote the awareness of and practice of mental health activities. At Love, NUSC, we believe that good mental health is a key to general well-being, and to that end, we endeavour to promote mental wellness in the community.</t>
-  </si>
-  <si>
-    <t>Every few weeks</t>
-  </si>
-  <si>
-    <t>Love, USP</t>
-  </si>
-  <si>
-    <t>Moodboard, Mental health and USP related dialogue and speaker sessions</t>
-  </si>
-  <si>
-    <t>Joshua Koh Ze Shao</t>
-  </si>
-  <si>
-    <t>joshua_kzs</t>
-  </si>
-  <si>
-    <t>joshuakzs@u.nus.edu</t>
-  </si>
-  <si>
-    <t>NUSC Astronomical Society</t>
-  </si>
-  <si>
-    <t>An astronomy-based interest group that mainly conducts star-gazing activities at night. The interest group will also provide knowledge to members about the different constellations seen at night and share random facts about our night sky. On occasions where eclipses may be observed, members of the interest group would also gather round to observe and document the sight. This interest group is a continuation of a University Scholars Programme interest group called UStronomy.</t>
-  </si>
-  <si>
-    <t>Whenever the sky looks clear enough to star gaze</t>
-  </si>
-  <si>
-    <t>UStronomy</t>
-  </si>
-  <si>
-    <t>https://t.me/joinchat/k07RzjszkIsyODU1</t>
-  </si>
-  <si>
-    <t>Aldwin Chia Kun Han</t>
-  </si>
-  <si>
-    <t>e0773080@u.nus.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUSC Fellowship </t>
-  </si>
-  <si>
-    <t>As a continuation of USFellowship, the USP Christian Fellowship IG, NUSC Fellowship aims to be a community for Christians in NUSC to study the Bible and find support, and for those seeking to find out more about Christianity to explore the faith.</t>
-  </si>
-  <si>
-    <t>Weekly small groups or IG-wide events, additional external speaker events or get-togethers</t>
-  </si>
-  <si>
-    <t>USFellowship</t>
-  </si>
-  <si>
-    <t>Bible/book studies, worship nights, prayer meetings, sharing by USP profs, Apologetics session</t>
-  </si>
-  <si>
-    <t>https://t.me/+Vmf1PYIiALJlMjJl</t>
-  </si>
-  <si>
-    <t>NUSC Invests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We are an IG for students to familiarize better with investing, build knowledge on financial literacy, and build skills for those who would like a career in the invest sector.                       NUSC Invests is an interest group for anyone/everyone who are interested in investing. It is a continuation of a USP interest group: US Invest. NUSC Invests does not provide financial advice, but rather creates a vibrant community that discusses the financial market (stocks, bonds, EFTs, and crypto). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock Analysis/ Virtual Portofolio Management/Movie screenings/etc.           Adhoc </t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Invest. </t>
   </si>
   <si>
     <t>https://t.me/+U2yBepj9jMg2ZDM1</t>
@@ -1261,10 +1261,7 @@
     <t>Similar to YNC Hacks</t>
   </si>
   <si>
-    <t>Main Discord Group:
-https://discord.gg/nvedymjC
-Telegram (Announcements):
-https://t.me/+U-2DfFT744Y5ZWZk</t>
+    <t>https://t.me/+U-2DfFT744Y5ZWZk</t>
   </si>
   <si>
     <t>Ng Wei Ming
@@ -1619,9 +1616,6 @@
     <t>Weekly trainings and nigh scrimmage, End-of-Sem tourneys, ICG, IFG</t>
   </si>
   <si>
-    <t>Contact IG Heads (Jonathan/ Jia Lin)</t>
-  </si>
-  <si>
     <t>Lynette, Han Bin</t>
   </si>
   <si>
@@ -1681,8 +1675,7 @@
     <t>Weekly trainings, ICG, friendlies with other RCs and Halls</t>
   </si>
   <si>
-    <t>https://t.me/+ISJuP8by4ZhkN2Rl (W)
-https://t.me/+iXE6OmjhFFBkMzI1(M)</t>
+    <t>https://t.me/+ISJuP8by4ZhkN2Rl</t>
   </si>
   <si>
     <t>Rachel Tan Rui En (W), Darren Ang (M)</t>
@@ -2120,7 +2113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2205,6 +2198,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2275,10 +2275,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2381,8 +2382,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2797,10 +2802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -2841,9 +2846,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="35.25">
+    <row r="3" spans="1:5" ht="36">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>11</v>
@@ -2857,12 +2862,12 @@
       </c>
       <c r="E3" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D3,Users!$B:$B, 0), 1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>11</v>
@@ -2871,17 +2876,17 @@
         <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH($B4,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
         <v>67</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D4,Users!$B:$B, 0), 1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>11</v>
@@ -2895,12 +2900,12 @@
       </c>
       <c r="E5" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D5,Users!$B:$B, 0), 1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>11</v>
@@ -2914,12 +2919,12 @@
       </c>
       <c r="E6" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D6,Users!$B:$B, 0), 1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
@@ -2933,12 +2938,12 @@
       </c>
       <c r="E7" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D7,Users!$B:$B, 0), 1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>11</v>
@@ -2952,12 +2957,12 @@
       </c>
       <c r="E8" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D8,Users!$B:$B, 0), 1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>11</v>
@@ -2971,12 +2976,12 @@
       </c>
       <c r="E9" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D9,Users!$B:$B, 0), 1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
@@ -2990,12 +2995,12 @@
       </c>
       <c r="E10" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D10,Users!$B:$B, 0), 1)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>11</v>
@@ -3009,12 +3014,12 @@
       </c>
       <c r="E11" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D11,Users!$B:$B, 0), 1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="36">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>11</v>
@@ -3028,12 +3033,12 @@
       </c>
       <c r="E12" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D12,Users!$B:$B, 0), 1)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="36">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>11</v>
@@ -3047,12 +3052,12 @@
       </c>
       <c r="E13" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D13,Users!$B:$B, 0), 1)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>11</v>
@@ -3066,12 +3071,12 @@
       </c>
       <c r="E14" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D14,Users!$B:$B, 0), 1)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="36">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
@@ -3085,12 +3090,12 @@
       </c>
       <c r="E15" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D15,Users!$B:$B, 0), 1)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="36">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>11</v>
@@ -3104,12 +3109,12 @@
       </c>
       <c r="E16" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D16,Users!$B:$B, 0), 1)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="36">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>11</v>
@@ -3123,12 +3128,12 @@
       </c>
       <c r="E17" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D17,Users!$B:$B, 0), 1)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="36">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>11</v>
@@ -3142,12 +3147,12 @@
       </c>
       <c r="E18" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D18,Users!$B:$B, 0), 1)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="36">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>11</v>
@@ -3161,12 +3166,12 @@
       </c>
       <c r="E19" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D19,Users!$B:$B, 0), 1)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="36">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>11</v>
@@ -3180,12 +3185,12 @@
       </c>
       <c r="E20" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D20,Users!$B:$B, 0), 1)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="36">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>11</v>
@@ -3199,25 +3204,6 @@
       </c>
       <c r="E21" s="6">
         <f>INDEX(Users!$A:$A, MATCH($D21,Users!$B:$B, 0), 1)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="36">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="6">
-        <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH($B22,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="6">
-        <f>INDEX(Users!$A:$A, MATCH($D22,Users!$B:$B, 0), 1)</f>
         <v>21</v>
       </c>
     </row>
@@ -3260,14 +3246,14 @@
         <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6">
         <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH($B4,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
         <v>66</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D2,'Test Users'!$B:$B, 0), 1)</f>
@@ -3287,7 +3273,7 @@
         <v>67</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D3,'Test Users'!$B:$B, 0), 1)</f>
@@ -3300,14 +3286,14 @@
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="6">
         <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH($B6,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
         <v>66</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D4,'Test Users'!$B:$B, 0), 1)</f>
@@ -3327,7 +3313,7 @@
         <v>67</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D5,'Test Users'!$B:$B, 0), 1)</f>
@@ -3340,14 +3326,14 @@
         <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="6">
         <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH($B8,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
         <v>66</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D6,'Test Users'!$B:$B, 0), 1)</f>
@@ -3367,7 +3353,7 @@
         <v>67</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D7,'Test Users'!$B:$B, 0), 1)</f>
@@ -3380,14 +3366,14 @@
         <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6">
         <f>INDEX('Organisations and IG Heads'!$A:$A, MATCH(B8,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
         <v>66</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D8,'Test Users'!$B:$B, 0), 1)</f>
@@ -3407,7 +3393,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="6">
         <f>INDEX('Test Users'!$A:$A, MATCH($D9,'Test Users'!$B:$B, 0), 1)</f>
@@ -3438,7 +3424,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.5">
@@ -3449,7 +3435,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.5">
@@ -3457,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>39</v>
@@ -3468,7 +3454,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>40</v>
@@ -3479,7 +3465,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -3490,7 +3476,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -3501,7 +3487,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -3512,7 +3498,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
@@ -3523,7 +3509,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
@@ -3534,7 +3520,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
@@ -3545,7 +3531,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
@@ -3556,7 +3542,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>48</v>
@@ -3567,7 +3553,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
@@ -3578,7 +3564,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>50</v>
@@ -3589,7 +3575,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -3600,7 +3586,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -3611,7 +3597,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>53</v>
@@ -3622,7 +3608,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>54</v>
@@ -3633,7 +3619,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
         <v>55</v>
@@ -3644,7 +3630,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>56</v>
@@ -3655,7 +3641,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
@@ -3666,7 +3652,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>58</v>
@@ -3699,7 +3685,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
@@ -3708,7 +3694,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>59</v>
@@ -3720,7 +3706,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>60</v>
@@ -3732,7 +3718,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>61</v>
@@ -3744,7 +3730,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>62</v>
@@ -3837,8 +3823,8 @@
   </sheetPr>
   <dimension ref="A1:AJ991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -4117,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>58</v>
@@ -4156,27 +4142,25 @@
       <c r="G6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J6" s="15">
         <v>0</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="20"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>97</v>
@@ -4190,25 +4174,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>136</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>93</v>
@@ -4217,17 +4201,17 @@
         <v>0</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R7" s="16" t="s">
         <v>97</v>
@@ -4241,44 +4225,42 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J8" s="15">
         <v>0</v>
       </c>
       <c r="K8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R8" s="16" t="s">
         <v>97</v>
@@ -4292,23 +4274,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>93</v>
@@ -4317,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>54</v>
@@ -4327,7 +4309,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R9" s="16" t="s">
         <v>97</v>
@@ -4341,25 +4323,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>156</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="18" t="s">
         <v>159</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>93</v>
@@ -4368,17 +4350,17 @@
         <v>0</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R10" s="16" t="s">
         <v>97</v>
@@ -4392,22 +4374,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>165</v>
@@ -4458,7 +4440,7 @@
         <v>110</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>172</v>
@@ -4713,7 +4695,7 @@
         <v>110</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>213</v>
@@ -4766,11 +4748,9 @@
       <c r="G18" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="4"/>
+      <c r="I18" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J18" s="15">
         <v>0</v>
@@ -4913,9 +4893,7 @@
       <c r="G21" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="H21" s="4"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15">
         <v>0</v>
@@ -4964,7 +4942,7 @@
         <v>252</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J22" s="15">
         <v>0</v>
@@ -5520,7 +5498,7 @@
         <v>340</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J33" s="15">
         <v>0</v>
@@ -5665,11 +5643,9 @@
       <c r="G36" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="4"/>
+      <c r="I36" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J36" s="15">
         <v>0</v>
@@ -5716,7 +5692,7 @@
       <c r="G37" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="38" t="s">
         <v>370</v>
       </c>
       <c r="I37" s="15" t="s">
@@ -5774,7 +5750,7 @@
         <v>379</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J38" s="15">
         <v>0</v>
@@ -6349,31 +6325,29 @@
       <c r="G50" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>486</v>
-      </c>
+      <c r="H50" s="4"/>
       <c r="I50" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J50" s="15">
         <v>0</v>
       </c>
       <c r="K50" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>487</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>488</v>
       </c>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="29"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="20" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="S50" s="25"/>
       <c r="T50" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="14.25" customHeight="1">
@@ -6381,25 +6355,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="24" t="s">
+        <v>490</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>491</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>492</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>401</v>
       </c>
       <c r="E51" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="H51" s="18" t="s">
         <v>495</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>496</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>93</v>
@@ -6408,21 +6382,21 @@
         <v>0</v>
       </c>
       <c r="K51" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="L51" s="15" t="s">
         <v>497</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>498</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
       <c r="O51" s="30"/>
       <c r="P51" s="15"/>
       <c r="Q51" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="S51" s="25"/>
       <c r="T51" s="37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="14.25" customHeight="1">
@@ -6430,25 +6404,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="24" t="s">
+        <v>500</v>
+      </c>
+      <c r="C52" s="13" t="s">
         <v>501</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>502</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>401</v>
       </c>
       <c r="E52" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="H52" s="38" t="s">
         <v>505</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>506</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>93</v>
@@ -6457,21 +6431,21 @@
         <v>0</v>
       </c>
       <c r="K52" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="L52" s="15" t="s">
         <v>507</v>
-      </c>
-      <c r="L52" s="15" t="s">
-        <v>508</v>
       </c>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
       <c r="P52" s="15"/>
       <c r="Q52" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="S52" s="25"/>
       <c r="T52" s="37" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="14.25" customHeight="1">
@@ -6479,25 +6453,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="24" t="s">
+        <v>510</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>511</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>512</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E53" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="G53" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="H53" s="18" t="s">
         <v>515</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>516</v>
       </c>
       <c r="I53" s="15" t="s">
         <v>93</v>
@@ -6506,17 +6480,17 @@
         <v>0</v>
       </c>
       <c r="K53" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="L53" s="15" t="s">
         <v>517</v>
-      </c>
-      <c r="L53" s="15" t="s">
-        <v>518</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
       <c r="O53" s="32"/>
       <c r="P53" s="15"/>
       <c r="Q53" s="33" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="S53" s="25"/>
     </row>
@@ -6525,25 +6499,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="24" t="s">
+        <v>519</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>520</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>521</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>401</v>
       </c>
       <c r="E54" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="H54" s="18" t="s">
         <v>524</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>525</v>
       </c>
       <c r="I54" s="15" t="s">
         <v>93</v>
@@ -6552,21 +6526,21 @@
         <v>0</v>
       </c>
       <c r="K54" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="L54" s="15" t="s">
         <v>526</v>
-      </c>
-      <c r="L54" s="15" t="s">
-        <v>527</v>
       </c>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
       <c r="P54" s="15"/>
       <c r="Q54" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="S54" s="25"/>
       <c r="T54" s="37" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="14.25" customHeight="1">
@@ -6574,25 +6548,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="C55" s="13" t="s">
         <v>530</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>531</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>401</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="18" t="s">
         <v>534</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>535</v>
       </c>
       <c r="I55" s="15" t="s">
         <v>93</v>
@@ -6620,25 +6594,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="24" t="s">
+        <v>535</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>536</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>537</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>220</v>
       </c>
       <c r="G56" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="H56" s="18" t="s">
         <v>539</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>540</v>
       </c>
       <c r="I56" s="15" t="s">
         <v>93</v>
@@ -6647,17 +6621,17 @@
         <v>0</v>
       </c>
       <c r="K56" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="L56" s="15" t="s">
         <v>541</v>
-      </c>
-      <c r="L56" s="15" t="s">
-        <v>542</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
       <c r="O56" s="15"/>
       <c r="P56" s="15"/>
       <c r="Q56" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S56" s="25"/>
     </row>
@@ -6666,25 +6640,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>544</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>545</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>401</v>
       </c>
       <c r="E57" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="F57" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="G57" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="H57" s="18" t="s">
         <v>548</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>549</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>93</v>
@@ -6693,17 +6667,17 @@
         <v>0</v>
       </c>
       <c r="K57" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="L57" s="15" t="s">
         <v>550</v>
-      </c>
-      <c r="L57" s="15" t="s">
-        <v>551</v>
       </c>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
       <c r="O57" s="15"/>
       <c r="P57" s="15"/>
       <c r="Q57" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="S57" s="25"/>
     </row>
@@ -6712,25 +6686,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="C58" s="13" t="s">
         <v>553</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>554</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E58" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="G58" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="H58" s="18" t="s">
         <v>557</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>558</v>
       </c>
       <c r="I58" s="15" t="s">
         <v>93</v>
@@ -6739,17 +6713,17 @@
         <v>0</v>
       </c>
       <c r="K58" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="L58" s="15" t="s">
         <v>559</v>
-      </c>
-      <c r="L58" s="15" t="s">
-        <v>560</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
       <c r="O58" s="32"/>
       <c r="P58" s="15"/>
       <c r="Q58" s="33" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S58" s="25"/>
     </row>
@@ -6758,25 +6732,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="C59" s="13" t="s">
         <v>562</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>563</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E59" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="G59" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="H59" s="18" t="s">
         <v>566</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>567</v>
       </c>
       <c r="I59" s="15" t="s">
         <v>93</v>
@@ -6785,21 +6759,21 @@
         <v>0</v>
       </c>
       <c r="K59" s="15" t="s">
+        <v>567</v>
+      </c>
+      <c r="L59" s="15" t="s">
         <v>568</v>
-      </c>
-      <c r="L59" s="15" t="s">
-        <v>569</v>
       </c>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
       <c r="O59" s="15"/>
       <c r="P59" s="15"/>
       <c r="Q59" s="15" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="S59" s="25"/>
       <c r="T59" s="37" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="14.25" customHeight="1">
@@ -6807,25 +6781,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="C60" s="13" t="s">
         <v>572</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>573</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E60" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="G60" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="H60" s="18" t="s">
         <v>576</v>
-      </c>
-      <c r="H60" s="18" t="s">
-        <v>577</v>
       </c>
       <c r="I60" s="15" t="s">
         <v>93</v>
@@ -6834,17 +6808,17 @@
         <v>0</v>
       </c>
       <c r="K60" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="L60" s="4" t="s">
         <v>578</v>
-      </c>
-      <c r="L60" s="4" t="s">
-        <v>579</v>
       </c>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
       <c r="P60" s="4"/>
       <c r="Q60" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="S60" s="25"/>
     </row>
@@ -6853,25 +6827,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="C61" s="13" t="s">
         <v>581</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>582</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E61" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="F61" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" s="18" t="s">
         <v>585</v>
-      </c>
-      <c r="H61" s="18" t="s">
-        <v>586</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>93</v>
@@ -6880,17 +6854,17 @@
         <v>0</v>
       </c>
       <c r="K61" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="L61" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>588</v>
       </c>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
       <c r="Q61" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="S61" s="25"/>
     </row>
@@ -6899,25 +6873,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>590</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>591</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E62" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" s="18" t="s">
         <v>594</v>
-      </c>
-      <c r="H62" s="18" t="s">
-        <v>595</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>93</v>
@@ -6926,21 +6900,21 @@
         <v>0</v>
       </c>
       <c r="K62" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="L62" s="4" t="s">
         <v>596</v>
-      </c>
-      <c r="L62" s="4" t="s">
-        <v>597</v>
       </c>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
       <c r="P62" s="4"/>
       <c r="Q62" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="S62" s="25"/>
       <c r="T62" s="37" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="14.25" customHeight="1">
@@ -6948,25 +6922,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="C63" s="13" t="s">
         <v>600</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>601</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E63" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="G63" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="H63" s="18" t="s">
         <v>603</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>604</v>
       </c>
       <c r="I63" s="15" t="s">
         <v>93</v>
@@ -6975,17 +6949,17 @@
         <v>0</v>
       </c>
       <c r="K63" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="L63" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="L63" s="4" t="s">
-        <v>606</v>
       </c>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
       <c r="P63" s="4"/>
       <c r="Q63" s="4" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="S63" s="25"/>
     </row>
@@ -6994,25 +6968,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>608</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>609</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E64" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="H64" s="14" t="s">
         <v>610</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>611</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>93</v>
@@ -7021,21 +6995,21 @@
         <v>0</v>
       </c>
       <c r="K64" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="L64" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="L64" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="S64" s="25"/>
       <c r="T64" s="37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="14.25" customHeight="1">
@@ -7043,44 +7017,42 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>616</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>617</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F65" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H65" s="4"/>
+      <c r="I65" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I65" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="J65" s="15">
         <v>0</v>
       </c>
       <c r="K65" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="L65" s="4" t="s">
         <v>619</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>620</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S65" s="25"/>
     </row>
@@ -7089,25 +7061,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>622</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>623</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>401</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F66" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H66" s="14" t="s">
         <v>624</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>625</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>93</v>
@@ -7116,17 +7088,17 @@
         <v>0</v>
       </c>
       <c r="K66" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="L66" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="L66" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="S66" s="25"/>
     </row>
@@ -7135,26 +7107,24 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="D67" s="35" t="s">
         <v>88</v>
       </c>
       <c r="E67" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="F67" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="G67" t="s">
-        <v>127</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>127</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="H67" s="4"/>
       <c r="I67" s="15" t="s">
         <v>93</v>
       </c>
@@ -7165,10 +7135,10 @@
         <v>10</v>
       </c>
       <c r="L67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q67" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S67" s="25"/>
     </row>
@@ -7180,37 +7150,35 @@
         <v>11</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="D68" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E68" t="s">
+        <v>164</v>
+      </c>
+      <c r="F68" t="s">
+        <v>164</v>
+      </c>
+      <c r="G68" t="s">
+        <v>164</v>
+      </c>
+      <c r="H68" s="4"/>
+      <c r="I68" t="s">
         <v>629</v>
-      </c>
-      <c r="E68" t="s">
-        <v>127</v>
-      </c>
-      <c r="F68" t="s">
-        <v>127</v>
-      </c>
-      <c r="G68" t="s">
-        <v>127</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I68" t="s">
-        <v>630</v>
       </c>
       <c r="J68" s="15">
         <v>1</v>
       </c>
       <c r="K68" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="L68" t="s">
         <v>39</v>
       </c>
       <c r="Q68" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S68" s="25"/>
     </row>
@@ -7219,40 +7187,38 @@
         <v>68</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C69" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D69" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E69" t="s">
+        <v>164</v>
+      </c>
+      <c r="F69" t="s">
+        <v>164</v>
+      </c>
+      <c r="G69" t="s">
+        <v>164</v>
+      </c>
+      <c r="H69" s="4"/>
+      <c r="I69" t="s">
         <v>629</v>
-      </c>
-      <c r="E69" t="s">
-        <v>127</v>
-      </c>
-      <c r="F69" t="s">
-        <v>127</v>
-      </c>
-      <c r="G69" t="s">
-        <v>127</v>
-      </c>
-      <c r="H69" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I69" t="s">
-        <v>630</v>
       </c>
       <c r="J69" s="15">
         <v>0</v>
       </c>
       <c r="K69" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="L69" t="s">
         <v>631</v>
       </c>
-      <c r="L69" t="s">
-        <v>632</v>
-      </c>
       <c r="Q69" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S69" s="25"/>
     </row>
@@ -7261,40 +7227,38 @@
         <v>69</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C70" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D70" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E70" t="s">
+        <v>164</v>
+      </c>
+      <c r="F70" t="s">
+        <v>164</v>
+      </c>
+      <c r="G70" t="s">
+        <v>164</v>
+      </c>
+      <c r="H70" s="4"/>
+      <c r="I70" t="s">
         <v>629</v>
-      </c>
-      <c r="E70" t="s">
-        <v>127</v>
-      </c>
-      <c r="F70" t="s">
-        <v>127</v>
-      </c>
-      <c r="G70" t="s">
-        <v>127</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I70" t="s">
-        <v>630</v>
       </c>
       <c r="J70" s="15">
         <v>0</v>
       </c>
       <c r="K70" s="36" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L70" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q70" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S70" s="25"/>
     </row>
@@ -7303,40 +7267,38 @@
         <v>70</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C71" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D71" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E71" t="s">
+        <v>164</v>
+      </c>
+      <c r="F71" t="s">
+        <v>164</v>
+      </c>
+      <c r="G71" t="s">
+        <v>164</v>
+      </c>
+      <c r="H71" s="4"/>
+      <c r="I71" t="s">
         <v>629</v>
-      </c>
-      <c r="E71" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" t="s">
-        <v>127</v>
-      </c>
-      <c r="G71" t="s">
-        <v>127</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I71" t="s">
-        <v>630</v>
       </c>
       <c r="J71" s="15">
         <v>0</v>
       </c>
       <c r="K71" s="36" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L71" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q71" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S71" s="25"/>
     </row>
@@ -7345,40 +7307,38 @@
         <v>71</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C72" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D72" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E72" t="s">
+        <v>164</v>
+      </c>
+      <c r="F72" t="s">
+        <v>164</v>
+      </c>
+      <c r="G72" t="s">
+        <v>164</v>
+      </c>
+      <c r="H72" s="4"/>
+      <c r="I72" t="s">
         <v>629</v>
-      </c>
-      <c r="E72" t="s">
-        <v>127</v>
-      </c>
-      <c r="F72" t="s">
-        <v>127</v>
-      </c>
-      <c r="G72" t="s">
-        <v>127</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I72" t="s">
-        <v>630</v>
       </c>
       <c r="J72" s="15">
         <v>0</v>
       </c>
       <c r="K72" s="36" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="L72" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q72" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S72" s="25"/>
     </row>
@@ -7387,40 +7347,38 @@
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C73" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D73" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E73" t="s">
+        <v>164</v>
+      </c>
+      <c r="F73" t="s">
+        <v>164</v>
+      </c>
+      <c r="G73" t="s">
+        <v>164</v>
+      </c>
+      <c r="H73" s="4"/>
+      <c r="I73" t="s">
         <v>629</v>
-      </c>
-      <c r="E73" t="s">
-        <v>127</v>
-      </c>
-      <c r="F73" t="s">
-        <v>127</v>
-      </c>
-      <c r="G73" t="s">
-        <v>127</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I73" t="s">
-        <v>630</v>
       </c>
       <c r="J73" s="15">
         <v>0</v>
       </c>
       <c r="K73" s="36" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="L73" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q73" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S73" s="25"/>
     </row>
@@ -7429,40 +7387,38 @@
         <v>73</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C74" s="34" t="s">
         <v>204</v>
       </c>
       <c r="D74" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E74" t="s">
+        <v>164</v>
+      </c>
+      <c r="F74" t="s">
+        <v>164</v>
+      </c>
+      <c r="G74" t="s">
+        <v>164</v>
+      </c>
+      <c r="H74" s="4"/>
+      <c r="I74" t="s">
         <v>629</v>
-      </c>
-      <c r="E74" t="s">
-        <v>127</v>
-      </c>
-      <c r="F74" t="s">
-        <v>127</v>
-      </c>
-      <c r="G74" t="s">
-        <v>127</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I74" t="s">
-        <v>630</v>
       </c>
       <c r="J74" s="15">
         <v>0</v>
       </c>
       <c r="K74" s="36" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="L74" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q74" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S74" s="25"/>
     </row>
@@ -7477,22 +7433,20 @@
         <v>204</v>
       </c>
       <c r="D75" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E75" t="s">
+        <v>164</v>
+      </c>
+      <c r="F75" t="s">
+        <v>164</v>
+      </c>
+      <c r="G75" t="s">
+        <v>164</v>
+      </c>
+      <c r="H75" s="4"/>
+      <c r="I75" t="s">
         <v>629</v>
-      </c>
-      <c r="E75" t="s">
-        <v>127</v>
-      </c>
-      <c r="F75" t="s">
-        <v>127</v>
-      </c>
-      <c r="G75" t="s">
-        <v>127</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I75" t="s">
-        <v>630</v>
       </c>
       <c r="J75" s="15">
         <v>0</v>
@@ -7501,10 +7455,10 @@
         <v>9</v>
       </c>
       <c r="L75" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Q75" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="S75" s="25"/>
     </row>
@@ -13063,6 +13017,7 @@
     <hyperlink ref="H63" r:id="rId54" xr:uid="{00000000-0004-0000-0600-000035000000}"/>
     <hyperlink ref="H64" r:id="rId55" xr:uid="{00000000-0004-0000-0600-000036000000}"/>
     <hyperlink ref="H66" r:id="rId56" xr:uid="{00000000-0004-0000-0600-000037000000}"/>
+    <hyperlink ref="H37" r:id="rId57" xr:uid="{58E15D4B-F767-4AF4-9093-A194442B1F33}"/>
   </hyperlinks>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Update seed and IG_database
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26625"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAF22249-C04F-4B09-AA8D-37A246CCCC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16689EC8-4AE9-4DC0-8D42-043488EF62BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seeding Instruction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="687">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -113,37 +113,37 @@
     <t>Wyman</t>
   </si>
   <si>
-    <t>ERICA SOH KE MIN</t>
-  </si>
-  <si>
-    <t>ASHLEY LOW JIA SHUEN</t>
-  </si>
-  <si>
-    <t>WONG ZHI MIN, OLIVIA</t>
-  </si>
-  <si>
-    <t>DUANGPORN SIRIKULWATTANON</t>
-  </si>
-  <si>
-    <t>GILLIAN RAE ANG TIAN-EN</t>
-  </si>
-  <si>
-    <t>EU SHAE-ANNE</t>
-  </si>
-  <si>
-    <t>CRYSTAL PHUA</t>
-  </si>
-  <si>
-    <t>NGIOW HAN BIN</t>
-  </si>
-  <si>
-    <t>ALDWIN CHIA KUN HAN</t>
-  </si>
-  <si>
-    <t>HANNAH ONG SI EN</t>
-  </si>
-  <si>
-    <t>ARCHIT GOSWAMI</t>
+    <t>Erica Soh Ke Min</t>
+  </si>
+  <si>
+    <t>Ashley Low Jia Shuen</t>
+  </si>
+  <si>
+    <t>Wong Zhi Min, Olivia</t>
+  </si>
+  <si>
+    <t>Duangporn Sirikulwattanon</t>
+  </si>
+  <si>
+    <t>Gillian Rae Ang Tian-en</t>
+  </si>
+  <si>
+    <t>Eu Shae-Anne</t>
+  </si>
+  <si>
+    <t>Crystal Phua</t>
+  </si>
+  <si>
+    <t>Ngiow Han Bin</t>
+  </si>
+  <si>
+    <t>Aldwin Chia Kun Han</t>
+  </si>
+  <si>
+    <t>Hannah Ong Si En</t>
+  </si>
+  <si>
+    <t>Archit Goswami</t>
   </si>
   <si>
     <t>Zeyuan</t>
@@ -176,7 +176,7 @@
     <t>Pei Cheng Yi</t>
   </si>
   <si>
-    <t>cicadatears</t>
+    <t>chengyi123</t>
   </si>
   <si>
     <t>holygoats</t>
@@ -581,9 +581,6 @@
     <t>https://t.me/joinchat/k07RzjszkIsyODU1</t>
   </si>
   <si>
-    <t>Aldwin Chia Kun Han</t>
-  </si>
-  <si>
     <t>e0773080@u.nus.edu</t>
   </si>
   <si>
@@ -2237,7 +2234,7 @@
     <t>Gautham;Justin Rong;Abelona Chew;Zara;Chew Hong Jin;Ibrahim;Jun Ming;Tessa;Lydia;Qi Xuan;Pei Cheng Yi;Lucy ;Wilson;Qian Qian;Erika;Bella;Jun Yi</t>
   </si>
   <si>
-    <t>gauliao98;tintinmon;Abelonaaaaaa;tiredoftulips;sarrrdin;ibrahimisramos;jmgoh;tessaa_aa;lydio;qi_xuAnn;cicadatears;lucylucylucylucylucy;wilsonxiang;qianqianqianqian;Erikacarrots;bellsps;AdamJY</t>
+    <t>gauliao98;tintinmon;Abelonaaaaaa;tiredoftulips;sarrrdin;ibrahimisramos;jmgoh;tessaa_aa;lydio;qi_xuAnn;chengyi123;lucylucylucylucylucy;wilsonxiang;qianqianqianqian;Erikacarrots;bellsps;AdamJY</t>
   </si>
   <si>
     <t>isActive</t>
@@ -2957,7 +2954,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -3654,7 +3651,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -4078,8 +4075,8 @@
   </sheetPr>
   <dimension ref="A1:AL991"/>
   <sheetViews>
-    <sheetView topLeftCell="Q54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="K65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R76" sqref="R76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -4576,7 +4573,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>55</v>
@@ -4588,7 +4585,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T9" s="16" t="s">
         <v>101</v>
@@ -4602,25 +4599,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="18" t="s">
         <v>162</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>97</v>
@@ -4655,25 +4652,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>164</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>165</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>97</v>
@@ -4682,10 +4679,10 @@
         <v>0</v>
       </c>
       <c r="K11" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -4694,7 +4691,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T11" s="16" t="s">
         <v>101</v>
@@ -4708,25 +4705,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>173</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>174</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>97</v>
@@ -4735,10 +4732,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -4747,7 +4744,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T12" s="16" t="s">
         <v>101</v>
@@ -4761,25 +4758,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>181</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>97</v>
@@ -4788,10 +4785,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -4800,7 +4797,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T13" s="16" t="s">
         <v>101</v>
@@ -4814,25 +4811,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>188</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>189</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>191</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>192</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>97</v>
@@ -4841,10 +4838,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -4853,7 +4850,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T14" s="16" t="s">
         <v>101</v>
@@ -4867,25 +4864,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>197</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>97</v>
@@ -4894,10 +4891,10 @@
         <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -4906,7 +4903,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T15" s="16" t="s">
         <v>101</v>
@@ -4920,25 +4917,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>205</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>206</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>210</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>97</v>
@@ -4947,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -4959,7 +4956,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T16" s="16" t="s">
         <v>101</v>
@@ -4973,25 +4970,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>214</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>215</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>97</v>
@@ -5000,10 +4997,10 @@
         <v>0</v>
       </c>
       <c r="K17" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>219</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -5012,7 +5009,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T17" s="16" t="s">
         <v>101</v>
@@ -5026,22 +5023,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>222</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F18" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="15" t="s">
@@ -5051,10 +5048,10 @@
         <v>0</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -5063,7 +5060,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T18" s="16"/>
       <c r="U18" s="17"/>
@@ -5073,25 +5070,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>228</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>229</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>231</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>97</v>
@@ -5100,10 +5097,10 @@
         <v>0</v>
       </c>
       <c r="K19" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -5112,7 +5109,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T19" s="16" t="s">
         <v>101</v>
@@ -5126,25 +5123,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>236</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>237</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="18" t="s">
         <v>240</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>241</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>97</v>
@@ -5153,10 +5150,10 @@
         <v>0</v>
       </c>
       <c r="K20" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>243</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -5165,7 +5162,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T20" s="16" t="s">
         <v>101</v>
@@ -5179,20 +5176,20 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>245</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>246</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="15"/>
@@ -5200,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="K21" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -5212,7 +5209,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T21" s="16" t="s">
         <v>101</v>
@@ -5226,23 +5223,23 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>253</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="18" t="s">
         <v>255</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>256</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>131</v>
@@ -5251,23 +5248,23 @@
         <v>0</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="13"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="R22" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="S22" s="13" t="s">
         <v>259</v>
-      </c>
-      <c r="S22" s="13" t="s">
-        <v>260</v>
       </c>
       <c r="T22" s="16" t="s">
         <v>101</v>
@@ -5281,25 +5278,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>262</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="18" t="s">
         <v>265</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>266</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>97</v>
@@ -5308,10 +5305,10 @@
         <v>0</v>
       </c>
       <c r="K23" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -5320,7 +5317,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T23" s="16" t="s">
         <v>101</v>
@@ -5334,25 +5331,25 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>271</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="18" t="s">
         <v>273</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>274</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>97</v>
@@ -5361,10 +5358,10 @@
         <v>0</v>
       </c>
       <c r="K24" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>276</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -5373,7 +5370,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T24" s="16" t="s">
         <v>101</v>
@@ -5387,25 +5384,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>278</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>279</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H25" s="22" t="s">
         <v>280</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>281</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>97</v>
@@ -5414,10 +5411,10 @@
         <v>0</v>
       </c>
       <c r="K25" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>283</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -5426,7 +5423,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T25" s="16" t="s">
         <v>101</v>
@@ -5440,25 +5437,25 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>285</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>286</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>288</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>289</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>97</v>
@@ -5467,10 +5464,10 @@
         <v>0</v>
       </c>
       <c r="K26" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>291</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -5479,7 +5476,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T26" s="16" t="s">
         <v>101</v>
@@ -5493,23 +5490,23 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>293</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>294</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>295</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>296</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>97</v>
@@ -5518,10 +5515,10 @@
         <v>0</v>
       </c>
       <c r="K27" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -5530,7 +5527,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T27" s="16" t="s">
         <v>101</v>
@@ -5544,25 +5541,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>300</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>301</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E28" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="G28" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H28" s="18" t="s">
         <v>303</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>304</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>97</v>
@@ -5571,10 +5568,10 @@
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>306</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -5583,7 +5580,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T28" s="16" t="s">
         <v>101</v>
@@ -5597,25 +5594,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>308</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>309</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H29" s="18" t="s">
         <v>310</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>311</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>97</v>
@@ -5624,10 +5621,10 @@
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L29" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>313</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -5636,7 +5633,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
       <c r="S29" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T29" s="16" t="s">
         <v>101</v>
@@ -5650,37 +5647,37 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>315</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>316</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="I30" s="15" t="s">
         <v>320</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>321</v>
       </c>
       <c r="J30" s="15">
         <v>0</v>
       </c>
       <c r="K30" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="L30" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>323</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -5689,7 +5686,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T30" s="16" t="s">
         <v>101</v>
@@ -5703,25 +5700,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>325</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>326</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F31" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="14" t="s">
         <v>328</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>329</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>97</v>
@@ -5730,10 +5727,10 @@
         <v>0</v>
       </c>
       <c r="K31" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="L31" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>331</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -5742,7 +5739,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="T31" s="16" t="s">
         <v>101</v>
@@ -5756,21 +5753,21 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>333</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>334</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>97</v>
@@ -5779,10 +5776,10 @@
         <v>0</v>
       </c>
       <c r="K32" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="L32" s="23" t="s">
         <v>337</v>
-      </c>
-      <c r="L32" s="23" t="s">
-        <v>338</v>
       </c>
       <c r="M32" s="23"/>
       <c r="N32" s="23"/>
@@ -5791,7 +5788,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="23"/>
       <c r="S32" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="T32" s="16" t="s">
         <v>101</v>
@@ -5805,23 +5802,23 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>340</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>341</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>343</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>131</v>
@@ -5830,10 +5827,10 @@
         <v>0</v>
       </c>
       <c r="K33" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="L33" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>346</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -5842,7 +5839,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="T33" s="16" t="s">
         <v>101</v>
@@ -5856,23 +5853,23 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="H34" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>351</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>97</v>
@@ -5881,10 +5878,10 @@
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="L34" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -5893,7 +5890,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="T34" s="16" t="s">
         <v>101</v>
@@ -5907,23 +5904,23 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>355</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>356</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="H35" s="18" t="s">
         <v>358</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>359</v>
       </c>
       <c r="I35" s="15" t="s">
         <v>97</v>
@@ -5932,10 +5929,10 @@
         <v>0</v>
       </c>
       <c r="K35" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="L35" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>361</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -5944,7 +5941,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
       <c r="S35" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="T35" s="16" t="s">
         <v>101</v>
@@ -5958,22 +5955,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>363</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>364</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="15" t="s">
@@ -5983,10 +5980,10 @@
         <v>0</v>
       </c>
       <c r="K36" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="L36" s="4" t="s">
         <v>367</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>368</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -5995,7 +5992,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="T36" s="16" t="s">
         <v>101</v>
@@ -6009,25 +6006,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>370</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>371</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H37" s="38" t="s">
         <v>373</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H37" s="38" t="s">
-        <v>374</v>
       </c>
       <c r="I37" s="15" t="s">
         <v>97</v>
@@ -6036,23 +6033,23 @@
         <v>0</v>
       </c>
       <c r="K37" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="L37" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>376</v>
       </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="R37" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="S37" s="4" t="s">
-        <v>379</v>
       </c>
       <c r="T37" s="16" t="s">
         <v>101</v>
@@ -6067,25 +6064,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>380</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>381</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="G38" s="4" t="s">
+      <c r="H38" s="18" t="s">
         <v>383</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>384</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>131</v>
@@ -6094,10 +6091,10 @@
         <v>0</v>
       </c>
       <c r="K38" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="L38" s="4" t="s">
         <v>385</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>386</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -6106,7 +6103,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
       <c r="S38" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="T38" s="16" t="s">
         <v>101</v>
@@ -6120,25 +6117,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>388</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>389</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H39" s="18" t="s">
         <v>391</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>392</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>97</v>
@@ -6147,10 +6144,10 @@
         <v>0</v>
       </c>
       <c r="K39" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="L39" s="4" t="s">
         <v>393</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>394</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -6159,7 +6156,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
       <c r="S39" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="T39" s="16" t="s">
         <v>101</v>
@@ -6173,25 +6170,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>396</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>397</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G40" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="H40" s="18" t="s">
         <v>398</v>
-      </c>
-      <c r="H40" s="18" t="s">
-        <v>399</v>
       </c>
       <c r="I40" s="15" t="s">
         <v>97</v>
@@ -6200,23 +6197,23 @@
         <v>0</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>400</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>401</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="R40" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="R40" s="4" t="s">
+      <c r="S40" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="S40" s="4" t="s">
-        <v>404</v>
       </c>
       <c r="T40" s="16" t="s">
         <v>101</v>
@@ -6231,23 +6228,23 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D41" s="15" t="s">
         <v>406</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>407</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="H41" s="18" t="s">
         <v>409</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>410</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>97</v>
@@ -6256,10 +6253,10 @@
         <v>0</v>
       </c>
       <c r="K41" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="L41" s="15" t="s">
         <v>411</v>
-      </c>
-      <c r="L41" s="15" t="s">
-        <v>412</v>
       </c>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
@@ -6270,7 +6267,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T41" s="16"/>
       <c r="U41" s="17"/>
@@ -6280,25 +6277,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="D42" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="H42" s="18" t="s">
         <v>418</v>
-      </c>
-      <c r="H42" s="18" t="s">
-        <v>419</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>97</v>
@@ -6307,10 +6304,10 @@
         <v>0</v>
       </c>
       <c r="K42" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="L42" s="15" t="s">
         <v>420</v>
-      </c>
-      <c r="L42" s="15" t="s">
-        <v>421</v>
       </c>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
@@ -6319,7 +6316,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
       <c r="S42" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T42" s="16"/>
       <c r="U42" s="17"/>
@@ -6329,25 +6326,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="24" t="s">
+        <v>422</v>
+      </c>
+      <c r="C43" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="D43" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" s="14" t="s">
         <v>427</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>428</v>
       </c>
       <c r="I43" s="15" t="s">
         <v>97</v>
@@ -6356,10 +6353,10 @@
         <v>0</v>
       </c>
       <c r="K43" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="L43" s="15" t="s">
         <v>429</v>
-      </c>
-      <c r="L43" s="15" t="s">
-        <v>430</v>
       </c>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -6370,7 +6367,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
       <c r="S43" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U43" s="25"/>
     </row>
@@ -6379,25 +6376,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="D44" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="H44" s="18" t="s">
         <v>436</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>437</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>97</v>
@@ -6406,23 +6403,23 @@
         <v>0</v>
       </c>
       <c r="K44" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="L44" s="15" t="s">
         <v>438</v>
-      </c>
-      <c r="L44" s="15" t="s">
-        <v>439</v>
       </c>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="R44" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="R44" s="15" t="s">
+      <c r="S44" s="15" t="s">
         <v>441</v>
-      </c>
-      <c r="S44" s="15" t="s">
-        <v>442</v>
       </c>
       <c r="U44" s="25"/>
       <c r="V44" s="37"/>
@@ -6432,25 +6429,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="D45" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" s="18" t="s">
         <v>447</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>448</v>
       </c>
       <c r="I45" s="15" t="s">
         <v>97</v>
@@ -6459,10 +6456,10 @@
         <v>0</v>
       </c>
       <c r="K45" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="L45" s="15" t="s">
         <v>449</v>
-      </c>
-      <c r="L45" s="15" t="s">
-        <v>450</v>
       </c>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -6471,7 +6468,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
       <c r="S45" s="15" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="U45" s="25"/>
     </row>
@@ -6480,25 +6477,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="24" t="s">
+        <v>451</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="D46" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="D46" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" s="18" t="s">
         <v>456</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>457</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>97</v>
@@ -6507,10 +6504,10 @@
         <v>0</v>
       </c>
       <c r="K46" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="L46" s="15" t="s">
         <v>458</v>
-      </c>
-      <c r="L46" s="15" t="s">
-        <v>459</v>
       </c>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -6519,7 +6516,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="U46" s="25"/>
     </row>
@@ -6528,23 +6525,23 @@
         <v>46</v>
       </c>
       <c r="B47" s="24" t="s">
+        <v>460</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>462</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="H47" s="18" t="s">
         <v>464</v>
-      </c>
-      <c r="H47" s="18" t="s">
-        <v>465</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>97</v>
@@ -6553,23 +6550,23 @@
         <v>0</v>
       </c>
       <c r="K47" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="L47" s="4" t="s">
         <v>466</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>467</v>
       </c>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="26"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="R47" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="R47" s="4" t="s">
+      <c r="S47" s="20" t="s">
         <v>469</v>
-      </c>
-      <c r="S47" s="20" t="s">
-        <v>470</v>
       </c>
       <c r="U47" s="25"/>
       <c r="V47" s="37"/>
@@ -6579,25 +6576,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="24" t="s">
+        <v>470</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>471</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="D48" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" s="18" t="s">
         <v>475</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>476</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>97</v>
@@ -6606,10 +6603,10 @@
         <v>0</v>
       </c>
       <c r="K48" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="L48" s="15" t="s">
         <v>477</v>
-      </c>
-      <c r="L48" s="15" t="s">
-        <v>478</v>
       </c>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -6618,7 +6615,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="U48" s="25"/>
     </row>
@@ -6627,23 +6624,23 @@
         <v>48</v>
       </c>
       <c r="B49" s="24" t="s">
+        <v>479</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>481</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" s="27" t="s">
         <v>483</v>
-      </c>
-      <c r="H49" s="27" t="s">
-        <v>484</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>97</v>
@@ -6652,23 +6649,23 @@
         <v>0</v>
       </c>
       <c r="K49" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="L49" s="4" t="s">
         <v>485</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>486</v>
       </c>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="28"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="R49" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="R49" s="4" t="s">
+      <c r="S49" s="4" t="s">
         <v>488</v>
-      </c>
-      <c r="S49" s="4" t="s">
-        <v>489</v>
       </c>
       <c r="U49" s="25"/>
       <c r="V49" s="37"/>
@@ -6678,22 +6675,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="24" t="s">
+        <v>489</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>491</v>
       </c>
-      <c r="D50" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>493</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>494</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="15" t="s">
@@ -6703,23 +6700,23 @@
         <v>0</v>
       </c>
       <c r="K50" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>496</v>
       </c>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="29"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="R50" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="R50" s="4" t="s">
+      <c r="S50" s="20" t="s">
         <v>498</v>
-      </c>
-      <c r="S50" s="20" t="s">
-        <v>499</v>
       </c>
       <c r="U50" s="25"/>
       <c r="V50" s="37"/>
@@ -6729,25 +6726,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="24" t="s">
+        <v>499</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>500</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="D51" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="D51" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="G51" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="H51" s="18" t="s">
         <v>504</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>505</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>97</v>
@@ -6756,23 +6753,23 @@
         <v>0</v>
       </c>
       <c r="K51" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="L51" s="15" t="s">
         <v>506</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>507</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
       <c r="O51" s="30"/>
       <c r="P51" s="15"/>
       <c r="Q51" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="R51" s="15" t="s">
         <v>508</v>
       </c>
-      <c r="R51" s="15" t="s">
+      <c r="S51" s="31" t="s">
         <v>509</v>
-      </c>
-      <c r="S51" s="31" t="s">
-        <v>510</v>
       </c>
       <c r="U51" s="25"/>
       <c r="V51" s="37"/>
@@ -6782,25 +6779,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="24" t="s">
+        <v>510</v>
+      </c>
+      <c r="C52" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="D52" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="D52" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="H52" s="38" t="s">
         <v>515</v>
-      </c>
-      <c r="H52" s="38" t="s">
-        <v>516</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>97</v>
@@ -6809,23 +6806,23 @@
         <v>0</v>
       </c>
       <c r="K52" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="L52" s="15" t="s">
         <v>517</v>
-      </c>
-      <c r="L52" s="15" t="s">
-        <v>518</v>
       </c>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
       <c r="P52" s="15"/>
       <c r="Q52" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="R52" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="R52" s="15" t="s">
+      <c r="S52" s="4" t="s">
         <v>520</v>
-      </c>
-      <c r="S52" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="U52" s="25"/>
       <c r="V52" s="37"/>
@@ -6835,25 +6832,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="24" t="s">
+        <v>521</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="D53" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E53" s="13" t="s">
         <v>523</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E53" s="13" t="s">
+      <c r="F53" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="G53" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="H53" s="18" t="s">
         <v>526</v>
-      </c>
-      <c r="H53" s="18" t="s">
-        <v>527</v>
       </c>
       <c r="I53" s="15" t="s">
         <v>97</v>
@@ -6862,10 +6859,10 @@
         <v>0</v>
       </c>
       <c r="K53" s="15" t="s">
+        <v>527</v>
+      </c>
+      <c r="L53" s="15" t="s">
         <v>528</v>
-      </c>
-      <c r="L53" s="15" t="s">
-        <v>529</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -6873,7 +6870,7 @@
       <c r="P53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="U53" s="25"/>
     </row>
@@ -6882,25 +6879,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="D54" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D54" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E54" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="G54" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="H54" s="18" t="s">
         <v>535</v>
-      </c>
-      <c r="H54" s="18" t="s">
-        <v>536</v>
       </c>
       <c r="I54" s="15" t="s">
         <v>97</v>
@@ -6909,23 +6906,23 @@
         <v>0</v>
       </c>
       <c r="K54" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="L54" s="15" t="s">
         <v>537</v>
-      </c>
-      <c r="L54" s="15" t="s">
-        <v>538</v>
       </c>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
       <c r="P54" s="15"/>
       <c r="Q54" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="R54" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="R54" s="15" t="s">
+      <c r="S54" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="S54" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="U54" s="25"/>
       <c r="V54" s="37"/>
@@ -6935,25 +6932,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="24" t="s">
+        <v>541</v>
+      </c>
+      <c r="C55" s="13" t="s">
         <v>542</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="D55" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="D55" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="F55" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="G55" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="18" t="s">
         <v>546</v>
-      </c>
-      <c r="H55" s="18" t="s">
-        <v>547</v>
       </c>
       <c r="I55" s="15" t="s">
         <v>97</v>
@@ -6962,10 +6959,10 @@
         <v>0</v>
       </c>
       <c r="K55" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="L55" s="15" t="s">
         <v>305</v>
-      </c>
-      <c r="L55" s="15" t="s">
-        <v>306</v>
       </c>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
@@ -6974,7 +6971,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U55" s="25"/>
     </row>
@@ -6983,25 +6980,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>548</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="D56" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="F56" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G56" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G56" s="4" t="s">
+      <c r="H56" s="18" t="s">
         <v>551</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>552</v>
       </c>
       <c r="I56" s="15" t="s">
         <v>97</v>
@@ -7010,10 +7007,10 @@
         <v>0</v>
       </c>
       <c r="K56" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="L56" s="15" t="s">
         <v>553</v>
-      </c>
-      <c r="L56" s="15" t="s">
-        <v>554</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -7022,7 +7019,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="U56" s="25"/>
     </row>
@@ -7031,25 +7028,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="24" t="s">
+        <v>555</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="D57" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="F57" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="G57" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="H57" s="18" t="s">
         <v>560</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>561</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>97</v>
@@ -7058,10 +7055,10 @@
         <v>0</v>
       </c>
       <c r="K57" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="L57" s="15" t="s">
         <v>562</v>
-      </c>
-      <c r="L57" s="15" t="s">
-        <v>563</v>
       </c>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
@@ -7070,7 +7067,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="U57" s="25"/>
     </row>
@@ -7079,25 +7076,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="24" t="s">
+        <v>564</v>
+      </c>
+      <c r="C58" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="D58" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="F58" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="G58" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="H58" s="18" t="s">
         <v>569</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>570</v>
       </c>
       <c r="I58" s="15" t="s">
         <v>97</v>
@@ -7106,10 +7103,10 @@
         <v>0</v>
       </c>
       <c r="K58" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="L58" s="15" t="s">
         <v>571</v>
-      </c>
-      <c r="L58" s="15" t="s">
-        <v>572</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
@@ -7118,7 +7115,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U58" s="25"/>
     </row>
@@ -7127,25 +7124,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="24" t="s">
+        <v>573</v>
+      </c>
+      <c r="C59" s="13" t="s">
         <v>574</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="D59" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="F59" s="4" t="s">
         <v>576</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="G59" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="H59" s="18" t="s">
         <v>578</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>579</v>
       </c>
       <c r="I59" s="15" t="s">
         <v>97</v>
@@ -7154,23 +7151,23 @@
         <v>0</v>
       </c>
       <c r="K59" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="L59" s="15" t="s">
         <v>580</v>
-      </c>
-      <c r="L59" s="15" t="s">
-        <v>581</v>
       </c>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
       <c r="O59" s="15"/>
       <c r="P59" s="15"/>
       <c r="Q59" s="15" t="s">
+        <v>581</v>
+      </c>
+      <c r="R59" s="15" t="s">
         <v>582</v>
       </c>
-      <c r="R59" s="15" t="s">
+      <c r="S59" s="15" t="s">
         <v>583</v>
-      </c>
-      <c r="S59" s="15" t="s">
-        <v>584</v>
       </c>
       <c r="U59" s="25"/>
       <c r="V59" s="37"/>
@@ -7180,25 +7177,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="C60" s="13" t="s">
         <v>585</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="D60" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E60" s="4" t="s">
+      <c r="F60" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="G60" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="H60" s="18" t="s">
         <v>589</v>
-      </c>
-      <c r="H60" s="18" t="s">
-        <v>590</v>
       </c>
       <c r="I60" s="15" t="s">
         <v>97</v>
@@ -7207,10 +7204,10 @@
         <v>0</v>
       </c>
       <c r="K60" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="L60" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="L60" s="4" t="s">
-        <v>592</v>
       </c>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
@@ -7219,7 +7216,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
       <c r="S60" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="U60" s="25"/>
     </row>
@@ -7228,25 +7225,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="C61" s="13" t="s">
         <v>594</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="D61" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E61" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="G61" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" s="18" t="s">
         <v>598</v>
-      </c>
-      <c r="H61" s="18" t="s">
-        <v>599</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>97</v>
@@ -7255,10 +7252,10 @@
         <v>0</v>
       </c>
       <c r="K61" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="L61" s="4" t="s">
         <v>600</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>601</v>
       </c>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
@@ -7267,7 +7264,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
       <c r="S61" s="4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="U61" s="25"/>
     </row>
@@ -7276,25 +7273,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>603</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="D62" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="D62" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="G62" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" s="18" t="s">
         <v>607</v>
-      </c>
-      <c r="H62" s="18" t="s">
-        <v>608</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>97</v>
@@ -7303,23 +7300,23 @@
         <v>0</v>
       </c>
       <c r="K62" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="L62" s="4" t="s">
         <v>609</v>
-      </c>
-      <c r="L62" s="4" t="s">
-        <v>610</v>
       </c>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
       <c r="P62" s="4"/>
       <c r="Q62" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="R62" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="R62" s="4" t="s">
+      <c r="S62" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="S62" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="U62" s="25"/>
       <c r="V62" s="37"/>
@@ -7329,25 +7326,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C63" s="13" t="s">
         <v>614</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="D63" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E63" s="4" t="s">
+      <c r="F63" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="G63" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="H63" s="18" t="s">
         <v>617</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="H63" s="18" t="s">
-        <v>618</v>
       </c>
       <c r="I63" s="15" t="s">
         <v>97</v>
@@ -7356,10 +7353,10 @@
         <v>0</v>
       </c>
       <c r="K63" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="L63" s="4" t="s">
         <v>619</v>
-      </c>
-      <c r="L63" s="4" t="s">
-        <v>620</v>
       </c>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
@@ -7368,7 +7365,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
       <c r="S63" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="U63" s="25"/>
     </row>
@@ -7377,25 +7374,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>622</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="D64" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E64" s="4" t="s">
+      <c r="F64" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="H64" s="14" t="s">
         <v>624</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>625</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>97</v>
@@ -7404,23 +7401,23 @@
         <v>0</v>
       </c>
       <c r="K64" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="L64" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="L64" s="4" t="s">
-        <v>627</v>
       </c>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="R64" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="R64" s="4" t="s">
+      <c r="S64" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="S64" s="4" t="s">
-        <v>630</v>
       </c>
       <c r="U64" s="25"/>
       <c r="V64" s="37"/>
@@ -7430,22 +7427,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>631</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="D65" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>633</v>
-      </c>
       <c r="F65" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="15" t="s">
@@ -7455,10 +7452,10 @@
         <v>0</v>
       </c>
       <c r="K65" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="L65" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="L65" s="4" t="s">
-        <v>635</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
@@ -7467,7 +7464,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
       <c r="S65" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="U65" s="25"/>
     </row>
@@ -7476,25 +7473,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>637</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="D66" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="F66" s="4" t="s">
+      <c r="G66" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H66" s="14" t="s">
         <v>639</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>640</v>
       </c>
       <c r="I66" s="15" t="s">
         <v>97</v>
@@ -7503,10 +7500,10 @@
         <v>0</v>
       </c>
       <c r="K66" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="L66" s="4" t="s">
         <v>641</v>
-      </c>
-      <c r="L66" s="4" t="s">
-        <v>642</v>
       </c>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
@@ -7515,7 +7512,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
       <c r="S66" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="U66" s="25"/>
     </row>
@@ -7544,7 +7541,7 @@
         <v>38</v>
       </c>
       <c r="S67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U67" s="25"/>
     </row>
@@ -7557,11 +7554,11 @@
       </c>
       <c r="C68" s="34"/>
       <c r="D68" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J68" s="15">
         <v>1</v>
@@ -7573,7 +7570,7 @@
         <v>42</v>
       </c>
       <c r="S68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U68" s="25"/>
     </row>
@@ -7582,33 +7579,33 @@
         <v>68</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C69" s="34"/>
       <c r="D69" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J69" s="15">
         <v>0</v>
       </c>
       <c r="K69" s="36" t="s">
+        <v>646</v>
+      </c>
+      <c r="L69" t="s">
         <v>647</v>
       </c>
-      <c r="L69" t="s">
+      <c r="Q69" s="36" t="s">
         <v>648</v>
       </c>
-      <c r="Q69" s="36" t="s">
+      <c r="R69" t="s">
         <v>649</v>
       </c>
-      <c r="R69" t="s">
-        <v>650</v>
-      </c>
       <c r="S69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U69" s="25"/>
     </row>
@@ -7617,33 +7614,33 @@
         <v>69</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C70" s="34"/>
       <c r="D70" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J70" s="15">
         <v>0</v>
       </c>
       <c r="K70" s="36" t="s">
+        <v>651</v>
+      </c>
+      <c r="L70" t="s">
         <v>652</v>
       </c>
-      <c r="L70" t="s">
+      <c r="Q70" s="36" t="s">
         <v>653</v>
       </c>
-      <c r="Q70" s="36" t="s">
+      <c r="R70" t="s">
         <v>654</v>
       </c>
-      <c r="R70" t="s">
-        <v>655</v>
-      </c>
       <c r="S70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U70" s="25"/>
     </row>
@@ -7652,33 +7649,33 @@
         <v>70</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C71" s="34"/>
       <c r="D71" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J71" s="15">
         <v>0</v>
       </c>
       <c r="K71" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="L71" t="s">
         <v>657</v>
       </c>
-      <c r="L71" t="s">
+      <c r="Q71" s="36" t="s">
         <v>658</v>
       </c>
-      <c r="Q71" s="36" t="s">
+      <c r="R71" t="s">
         <v>659</v>
       </c>
-      <c r="R71" t="s">
-        <v>660</v>
-      </c>
       <c r="S71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U71" s="25"/>
     </row>
@@ -7687,33 +7684,33 @@
         <v>71</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C72" s="34"/>
       <c r="D72" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J72" s="15">
         <v>0</v>
       </c>
       <c r="K72" s="36" t="s">
+        <v>661</v>
+      </c>
+      <c r="L72" t="s">
         <v>662</v>
       </c>
-      <c r="L72" t="s">
+      <c r="Q72" s="36" t="s">
         <v>663</v>
       </c>
-      <c r="Q72" s="36" t="s">
+      <c r="R72" t="s">
         <v>664</v>
       </c>
-      <c r="R72" t="s">
-        <v>665</v>
-      </c>
       <c r="S72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U72" s="25"/>
     </row>
@@ -7722,33 +7719,33 @@
         <v>72</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C73" s="34"/>
       <c r="D73" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J73" s="15">
         <v>0</v>
       </c>
       <c r="K73" s="36" t="s">
+        <v>666</v>
+      </c>
+      <c r="L73" t="s">
         <v>667</v>
       </c>
-      <c r="L73" t="s">
+      <c r="Q73" s="36" t="s">
         <v>668</v>
       </c>
-      <c r="Q73" s="36" t="s">
+      <c r="R73" t="s">
         <v>669</v>
       </c>
-      <c r="R73" t="s">
-        <v>670</v>
-      </c>
       <c r="S73" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U73" s="25"/>
     </row>
@@ -7757,33 +7754,33 @@
         <v>73</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C74" s="34"/>
       <c r="D74" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J74" s="15">
         <v>0</v>
       </c>
       <c r="K74" s="36" t="s">
+        <v>671</v>
+      </c>
+      <c r="L74" t="s">
         <v>672</v>
       </c>
-      <c r="L74" t="s">
+      <c r="Q74" s="36" t="s">
         <v>673</v>
       </c>
-      <c r="Q74" s="36" t="s">
+      <c r="R74" t="s">
         <v>674</v>
       </c>
-      <c r="R74" t="s">
-        <v>675</v>
-      </c>
       <c r="S74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U74" s="25"/>
     </row>
@@ -7792,33 +7789,33 @@
         <v>74</v>
       </c>
       <c r="B75" s="36" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C75" s="34"/>
       <c r="D75" s="35" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="J75" s="15">
         <v>0</v>
       </c>
       <c r="K75" s="37" t="s">
+        <v>676</v>
+      </c>
+      <c r="L75" t="s">
         <v>677</v>
       </c>
-      <c r="L75" t="s">
+      <c r="Q75" s="36" t="s">
         <v>678</v>
       </c>
-      <c r="Q75" s="36" t="s">
+      <c r="R75" t="s">
         <v>679</v>
       </c>
-      <c r="R75" t="s">
-        <v>680</v>
-      </c>
       <c r="S75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="U75" s="25"/>
     </row>
@@ -13391,7 +13388,7 @@
   </sheetPr>
   <dimension ref="A1:AM918"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -13443,7 +13440,7 @@
         <v>78</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>79</v>
@@ -13503,13 +13500,13 @@
         <v>75</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>681</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>682</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>683</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
@@ -13517,7 +13514,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="38" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>97</v>
@@ -13529,10 +13526,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>686</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -13541,7 +13538,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="38" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U2" s="16" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Rename to isAdminOrg and fix routes
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26712"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B093B34-6E4F-4770-8749-21361DA53E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA8E6258-283F-4704-9502-7CBE42F50B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="7" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seeding Instruction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="708">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -299,7 +299,7 @@
     <t>How to Join</t>
   </si>
   <si>
-    <t>isOrganisationVerified</t>
+    <t>isAdminOrg</t>
   </si>
   <si>
     <t>isInvisible</t>
@@ -2300,6 +2300,9 @@
   </si>
   <si>
     <t>isInactive</t>
+  </si>
+  <si>
+    <t>isOrganisationVerified</t>
   </si>
   <si>
     <t>Inactive Test Group</t>
@@ -4204,8 +4207,8 @@
   </sheetPr>
   <dimension ref="A1:AM991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -13884,7 +13887,7 @@
         <v>700</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>79</v>
+        <v>701</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>80</v>
@@ -13944,10 +13947,10 @@
         <v>78</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>650</v>
@@ -13958,7 +13961,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="38" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>98</v>
@@ -13973,10 +13976,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -13985,7 +13988,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="38" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Update error message as per issue #74 on the frontend repo: https://github.com/usdevs/usc-website-hackathon-frontend/issues/74
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFFC8944-F454-4215-ABA5-DCCEB7746AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{939D8794-4996-4F61-8C90-B3C14F17B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="710">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -1124,7 +1124,7 @@
     <t>NUSCreatives</t>
   </si>
   <si>
-    <t>Objectives: - provide a safe space for budding writers of all levels to share their creative writing with one another - provide an organized time period for people to work on their creative writing endeavors - introduce a sense of professionalism to the writing process by having peer-advised editing and encouraging submitting works to literary journals - have a space for people to share their love for creative writing! :) - note: the writing can be in all languages, not just English! while sessions will be held in English, creation of non-English writing will require a translation from the author! - magazine part inspired by PLAYSET! Magazine.</t>
+    <t>We are a beginner-friendly IG dedicated to the art of creative writing. We welcome writers of all creative mediums and genres, regardless of level of experience. Love writing horror poems? Arthouse films? Or are you curious about the craft? Welcome to the club!</t>
   </si>
   <si>
     <t>PLAYSET! Magazine</t>
@@ -2291,9 +2291,6 @@
   </si>
   <si>
     <t>divno19</t>
-  </si>
-  <si>
-    <t>We are a beginner-friendly IG dedicated to the art of creative writing. We welcome writers of all creative mediums and genres, regardless of level of experience. Love writing horror poems? Arthouse films? Or are you curious about the craft? Welcome to the club!</t>
   </si>
   <si>
     <t>NUSC Poly! (Mentorship)</t>
@@ -4113,10 +4110,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL989"/>
+  <dimension ref="A1:AL988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75"/>
@@ -8132,11 +8129,9 @@
         <v>78</v>
       </c>
       <c r="B79" s="36" t="s">
-        <v>323</v>
-      </c>
-      <c r="C79" s="34" t="s">
         <v>698</v>
       </c>
+      <c r="C79" s="34"/>
       <c r="D79" s="35" t="s">
         <v>92</v>
       </c>
@@ -8150,39 +8145,17 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>328</v>
+        <v>699</v>
       </c>
       <c r="M79" t="s">
-        <v>329</v>
+        <v>700</v>
       </c>
       <c r="U79" s="25"/>
     </row>
     <row r="80" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A80" s="39">
-        <v>79</v>
-      </c>
-      <c r="B80" s="36" t="s">
-        <v>699</v>
-      </c>
+      <c r="B80" s="36"/>
       <c r="C80" s="34"/>
-      <c r="D80" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="I80" s="43" t="s">
-        <v>649</v>
-      </c>
-      <c r="J80" s="44">
-        <v>0</v>
-      </c>
-      <c r="K80" s="44">
-        <v>0</v>
-      </c>
-      <c r="L80" t="s">
-        <v>700</v>
-      </c>
-      <c r="M80" t="s">
-        <v>701</v>
-      </c>
+      <c r="D80" s="35"/>
       <c r="U80" s="25"/>
     </row>
     <row r="81" spans="2:21" ht="14.25" customHeight="1">
@@ -13616,9 +13589,6 @@
       <c r="U985" s="25"/>
     </row>
     <row r="986" spans="2:21" ht="14.25" customHeight="1">
-      <c r="B986" s="36"/>
-      <c r="C986" s="34"/>
-      <c r="D986" s="35"/>
       <c r="U986" s="25"/>
     </row>
     <row r="987" spans="2:21" ht="14.25" customHeight="1">
@@ -13626,9 +13596,6 @@
     </row>
     <row r="988" spans="2:21" ht="14.25" customHeight="1">
       <c r="U988" s="25"/>
-    </row>
-    <row r="989" spans="2:21" ht="14.25" customHeight="1">
-      <c r="U989" s="25"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -13764,10 +13731,10 @@
         <v>78</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>701</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>702</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>703</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>80</v>
@@ -13784,7 +13751,7 @@
         <v>83</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="S1" s="10" t="s">
         <v>84</v>
@@ -13824,13 +13791,13 @@
     <row r="2" spans="1:40" ht="95.25" customHeight="1">
       <c r="A2" s="4" cm="1">
         <f t="array" ref="A2">INDEX('Organisations and IG Heads'!$A:$A, COUNTA('Organisations and IG Heads'!$A:$A))+ROW()-1</f>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>705</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>706</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>648</v>
@@ -13841,7 +13808,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="38" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>97</v>
@@ -13856,10 +13823,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>709</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -13868,7 +13835,7 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="38" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
refactor: rename maker admin to spaces admin
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -2344,7 +2344,7 @@
     <t>e0123456@u.nus.edu</t>
   </si>
   <si>
-    <t>Maker Admin</t>
+    <t>Spaces Admin</t>
   </si>
   <si>
     <t>Aiken</t>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="B3" s="59" t="str">
         <f>'Test Organisations and IG Heads'!B3</f>
-        <v>Maker Admin</v>
+        <v>Spaces Admin</v>
       </c>
       <c r="C3" s="5">
         <f>'Test Organisations and IG Heads'!K3</f>

</xml_diff>

<commit_message>
feat: add member and dev users to excel
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheng\uscwebsite-hackathon-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDFB501-1C0A-47CA-AB7A-2BBE9FFB1BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A193C53-F513-44CF-93B1-ACE47F856877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24098" yWindow="-98" windowWidth="24196" windowHeight="14476" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23610" yWindow="390" windowWidth="18000" windowHeight="10553" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seeding Instruction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="748">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -2408,6 +2408,12 @@
   </si>
   <si>
     <t>buttery</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>dev</t>
   </si>
 </sst>
 </file>
@@ -8570,7 +8576,7 @@
       </c>
       <c r="D2" s="4">
         <f t="array" ref="D2">INDEX('Test Users'!$A:$A, MATCH($C2,'Test Users'!$B:$B, 0), 1)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -8589,7 +8595,7 @@
       </c>
       <c r="D3" s="4">
         <f t="array" ref="D3">INDEX('Test Users'!$A:$A, MATCH($C3,'Test Users'!$B:$B, 0), 1)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -8608,7 +8614,7 @@
       </c>
       <c r="D4" s="4">
         <f t="array" ref="D4">INDEX('Test Users'!$A:$A, MATCH($C4,'Test Users'!$B:$B, 0), 1)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4">
         <v>1</v>
@@ -8627,7 +8633,7 @@
       </c>
       <c r="D5" s="4">
         <f t="array" ref="D5">INDEX('Test Users'!$A:$A, MATCH($C5,'Test Users'!$B:$B, 0), 1)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -8646,7 +8652,7 @@
       </c>
       <c r="D6" s="4">
         <f t="array" ref="D6">INDEX('Test Users'!$A:$A, MATCH($C6,'Test Users'!$B:$B, 0), 1)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -8665,7 +8671,7 @@
       </c>
       <c r="D7" s="4">
         <f t="array" ref="D7">INDEX('Test Users'!$A:$A, MATCH($C7,'Test Users'!$B:$B, 0), 1)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -8684,7 +8690,7 @@
       </c>
       <c r="D8" s="4">
         <f t="array" ref="D8">INDEX('Test Users'!$A:$A, MATCH($C8,'Test Users'!$B:$B, 0), 1)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -8703,7 +8709,7 @@
       </c>
       <c r="D9" s="4">
         <f t="array" ref="D9">INDEX('Test Users'!$A:$A, MATCH($C9,'Test Users'!$B:$B, 0), 1)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
@@ -8722,7 +8728,7 @@
       </c>
       <c r="D10" s="4">
         <f t="array" ref="D10">INDEX('Test Users'!$A:$A, MATCH($C10,'Test Users'!$B:$B, 0), 1)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -9809,7 +9815,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10060,9 +10066,15 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="56">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="56"/>
@@ -11067,7 +11079,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11089,7 +11101,7 @@
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <f t="array" ref="A2">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>30</v>
@@ -11101,7 +11113,7 @@
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <f t="array" ref="A3">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>31</v>
@@ -11113,7 +11125,7 @@
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <f t="array" ref="A4">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>32</v>
@@ -11125,7 +11137,7 @@
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <f t="array" ref="A5">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>33</v>
@@ -11137,7 +11149,7 @@
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <f t="array" ref="A6">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>34</v>
@@ -11149,7 +11161,7 @@
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <f t="array" ref="A7">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>65</v>
@@ -11161,7 +11173,7 @@
     <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <f t="array" ref="A8">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>67</v>
@@ -11173,7 +11185,7 @@
     <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <f t="array" ref="A9">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>69</v>
@@ -11185,7 +11197,7 @@
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <f t="array" ref="A10">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>71</v>
@@ -11197,7 +11209,7 @@
     <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <f t="array" ref="A11">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>73</v>
@@ -11209,7 +11221,7 @@
     <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <f t="array" ref="A12">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>75</v>
@@ -11221,7 +11233,7 @@
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <f t="array" ref="A13">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>77</v>
@@ -11233,7 +11245,7 @@
     <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <f t="array" ref="A14">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>79</v>
@@ -11245,7 +11257,7 @@
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <f t="array" ref="A15">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>81</v>
@@ -11257,7 +11269,7 @@
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <f t="array" ref="A16">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>83</v>
@@ -11269,7 +11281,7 @@
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <f t="array" ref="A17">INDEX(Users!$A:$A, COUNTA(Users!$A:$A))+ROW()-1</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>85</v>
@@ -11279,8 +11291,15 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18">
+        <v>39</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
@@ -13381,7 +13400,7 @@
   <dimension ref="A1:AL1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>

</xml_diff>

<commit_message>
fix: update booking on behalf for RBAC
</commit_message>
<xml_diff>
--- a/IG_Database.xlsx
+++ b/IG_Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheng\uscwebsite-hackathon-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A193C53-F513-44CF-93B1-ACE47F856877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49C5531-A636-495D-909C-486A2E53A944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23610" yWindow="390" windowWidth="18000" windowHeight="10553" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seeding Instruction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="748">
   <si>
     <t>I've collated the data into Venues, Organisations and Users</t>
   </si>
@@ -4051,7 +4051,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
@@ -8536,8 +8536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8819,7 +8819,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="array" ref="B16">INDEX('Organisations and IG Heads'!$A:$A, MATCH(A16,'Organisations and IG Heads'!$B:$B, 0), 1)</f>
+        <v>67</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="array" ref="D16">INDEX('Test Users'!$A:$A, MATCH($C16,'Test Users'!$B:$B, 0), 1)</f>
+        <v>39</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9806,7 +9824,7 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11078,7 +11096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>